<commit_message>
2024/12/03 morning Signed-off-by: Annie <FengMu9966@gmail.com>
</commit_message>
<xml_diff>
--- a/document/StudyNotes/SqlStudyNotes/SqlDataTableNotes/後臺管理表/後臺資料表設計.xlsx
+++ b/document/StudyNotes/SqlStudyNotes/SqlDataTableNotes/後臺管理表/後臺資料表設計.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="63">
   <si>
     <t>KEY</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -83,10 +83,6 @@
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
-    <t>int</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
     <t>用戶狀態，1: 啟用，0: 禁用</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
@@ -112,14 +108,6 @@
   </si>
   <si>
     <t>identity</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>Y</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>varchar(10)</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
@@ -139,18 +127,10 @@
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
-    <t>描述權限</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
     <t>permission資料表(t_permission)</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>datetime</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
     <t>roles資料表(t_roles)</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -163,79 +143,27 @@
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
-    <t>數字</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>session資料表(t_session)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>identity</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>only one</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>f_sessionId</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>f_sid</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>f_updatedDate</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>f_createdDate</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>datetime</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>tinyint</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
     <t>f_roleId</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>N</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>對應的腳色名</t>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>f_roleId</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
-    <t>N</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>對應的腳色名</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>f_roleId</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
     <t>f_rolePermissionId</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>f_permissionId</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>f_permissionId</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>流水號</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
@@ -251,43 +179,87 @@
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
-    <t>varchar(80)</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
     <t>tinyint</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>流水號 unsigned</t>
+    <t>tinyint</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>f_account</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>f_name</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>varchar(20)</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>暱稱</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Y</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>bit</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>SHA-256長度為32 轉乘base64儲存 總長度:68</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>f_sessionId</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>varchar(128)</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Y</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>會話ID(登入了沒有)</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>varchar(101)</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">流水號 </t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
-    <t>tinyint</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>roles_permission資料表(t_roles_permission)</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>int</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>int</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>f_uid</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>角色名對應的數 unsigned</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>f_account</t>
+    <t>f_permissionId</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>f_roleId</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>varchar(60)</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>N</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>N</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>roles_permission資料表(t_rolePermission)</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
@@ -295,47 +267,23 @@
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
-    <t>varchar(20)</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>暱稱</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>Y</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>varchar(100)</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>bit</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>SHA-256長度為32 轉乘base64儲存 總長度:68</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>GETDATE()</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>f_sessionId</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>varchar(128)</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>Y</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>會話ID(登入了沒有)</t>
+    <t>varchar(30)</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>角色名字</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>INT</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>f_rolePermission</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>bigint</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
@@ -343,7 +291,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -395,14 +343,6 @@
       <name val="新細明體"/>
       <family val="2"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="新細明體"/>
-      <family val="1"/>
-      <charset val="136"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -497,7 +437,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -525,7 +465,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -536,9 +476,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -854,10 +791,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G43"/>
+  <dimension ref="A2:G35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
@@ -873,257 +810,261 @@
     <col min="12" max="12" width="24.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="12"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" s="5"/>
+      <c r="B5" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="2"/>
+      <c r="F5" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6" s="11"/>
-      <c r="C6" s="11"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="11"/>
-      <c r="F6" s="12"/>
+      <c r="A6" s="5"/>
+      <c r="B6" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="2"/>
+      <c r="F6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>5</v>
-      </c>
+      <c r="A7" s="8"/>
+      <c r="B7" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="E7" s="2"/>
+      <c r="F7" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="G7" s="7"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" s="3" t="s">
+      <c r="A8" s="6"/>
+      <c r="B8" s="4" t="s">
         <v>16</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>7</v>
+        <v>43</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E8" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>52</v>
+      <c r="E8" s="2">
+        <v>1</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" s="5"/>
-      <c r="B9" s="3" t="s">
-        <v>63</v>
+      <c r="A9" s="6"/>
+      <c r="B9" s="4" t="s">
+        <v>27</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>10</v>
+        <v>35</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>9</v>
+        <v>28</v>
       </c>
       <c r="E9" s="2"/>
       <c r="F9" s="3" t="s">
-        <v>11</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="G9" s="9"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" s="5"/>
-      <c r="B10" s="3" t="s">
-        <v>30</v>
+      <c r="A10" s="6"/>
+      <c r="B10" s="4" t="s">
+        <v>45</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>9</v>
+        <v>46</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>47</v>
       </c>
       <c r="E10" s="2"/>
       <c r="F10" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="G10" s="7" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" s="8"/>
-      <c r="B11" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="E11" s="2"/>
-      <c r="F11" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="G11" s="7"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" s="6"/>
-      <c r="B12" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="D12" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" s="11"/>
+      <c r="C13" s="11"/>
+      <c r="D13" s="11"/>
+      <c r="E13" s="11"/>
+      <c r="F13" s="12"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D15" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E12" s="2">
-        <v>1</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="G12" s="7" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" s="6"/>
-      <c r="B13" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="C13" s="3" t="s">
+      <c r="E15" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" s="5"/>
+      <c r="B16" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E16" s="2"/>
+      <c r="F16" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="G16" s="7"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17" s="5"/>
+      <c r="B17" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C17" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="D13" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="E13" s="2"/>
-      <c r="F13" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="G13" s="13"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" s="6"/>
-      <c r="B14" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="E14" s="2"/>
-      <c r="F14" s="3" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A17" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="B17" s="11"/>
-      <c r="C17" s="11"/>
-      <c r="D17" s="11"/>
-      <c r="E17" s="11"/>
-      <c r="F17" s="12"/>
+      <c r="D17" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E17" s="2"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="9"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A19" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F19" s="4" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A20" s="5"/>
-      <c r="B20" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E20" s="2"/>
-      <c r="F20" s="3" t="s">
+      <c r="A18" s="5"/>
+      <c r="B18" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C18" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="G20" s="7" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A21" s="5"/>
-      <c r="B21" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C21" s="3" t="s">
+      <c r="D18" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="D21" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E21" s="2"/>
-      <c r="F21" s="3"/>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A22" s="6"/>
-      <c r="B22" s="4"/>
-      <c r="C22" s="3"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
-      <c r="F22" s="3"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="3"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" s="10" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B24" s="11"/>
       <c r="C24" s="11"/>
@@ -1156,10 +1097,10 @@
         <v>6</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>57</v>
+        <v>37</v>
       </c>
       <c r="D26" s="2" t="s">
         <v>9</v>
@@ -1168,52 +1109,36 @@
         <v>8</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" s="5"/>
       <c r="B27" s="3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="D27" s="2" t="s">
         <v>9</v>
       </c>
       <c r="E27" s="2"/>
       <c r="F27" s="3" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" s="5"/>
-      <c r="B28" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="D28" s="5" t="s">
-        <v>9</v>
-      </c>
+      <c r="B28" s="3"/>
+      <c r="C28" s="3"/>
+      <c r="D28" s="5"/>
       <c r="E28" s="2"/>
-      <c r="F28" s="3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A29" s="6"/>
-      <c r="B29" s="4"/>
-      <c r="C29" s="3"/>
-      <c r="D29" s="2"/>
-      <c r="E29" s="2"/>
-      <c r="F29" s="3"/>
+      <c r="F28" s="3"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" s="10" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B31" s="11"/>
       <c r="C31" s="11"/>
@@ -1246,31 +1171,31 @@
         <v>6</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>47</v>
+        <v>31</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>12</v>
+        <v>60</v>
       </c>
       <c r="D33" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E33" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E33" s="2" t="s">
-        <v>19</v>
-      </c>
       <c r="F33" s="3" t="s">
-        <v>51</v>
+        <v>33</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" s="2"/>
       <c r="B34" s="3" t="s">
-        <v>46</v>
+        <v>30</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>53</v>
+        <v>35</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>20</v>
+        <v>55</v>
       </c>
       <c r="E34" s="2"/>
       <c r="F34" s="3"/>
@@ -1278,130 +1203,21 @@
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" s="5"/>
       <c r="B35" s="3" t="s">
-        <v>48</v>
+        <v>32</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>57</v>
+        <v>37</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>20</v>
+        <v>55</v>
       </c>
       <c r="E35" s="2"/>
       <c r="F35" s="3"/>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A37" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="B37" s="11"/>
-      <c r="C37" s="11"/>
-      <c r="D37" s="11"/>
-      <c r="E37" s="11"/>
-      <c r="F37" s="12"/>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A38" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C38" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D38" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E38" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F38" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A39" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B39" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="D39" s="1"/>
-      <c r="E39" s="1"/>
-      <c r="F39" s="9" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A40" s="2"/>
-      <c r="B40" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C40" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D40" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E40" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="F40" s="4" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A41" s="5"/>
-      <c r="B41" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="C41" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="D41" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E41" s="2"/>
-      <c r="F41" s="3"/>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A42" s="5"/>
-      <c r="B42" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="C42" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="D42" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E42" s="2"/>
-      <c r="F42" s="3"/>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A43" s="6"/>
-      <c r="B43" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="C43" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="D43" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E43" s="2"/>
-      <c r="F43" s="3" t="s">
-        <v>71</v>
-      </c>
-    </row>
   </sheetData>
-  <mergeCells count="5">
-    <mergeCell ref="A37:F37"/>
-    <mergeCell ref="A6:F6"/>
-    <mergeCell ref="A17:F17"/>
+  <mergeCells count="4">
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="A13:F13"/>
     <mergeCell ref="A24:F24"/>
     <mergeCell ref="A31:F31"/>
   </mergeCells>

</xml_diff>